<commit_message>
push for power issues
</commit_message>
<xml_diff>
--- a/Noncode documents/RF matrix.xlsx
+++ b/Noncode documents/RF matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike\Documents\GitHub\US-City-Climate-Change-Risk-and-Readiness\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike\Documents\GitHub\US-City-Climate-Change-Risk-and-Readiness\Noncode documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C192F815-C9AF-4E49-8F0A-0EFF2CFABF9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C4AB98-4988-4A11-92AA-6208F8CD9D27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{E222333D-3187-4F6C-B38B-685ECA80A3FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E222333D-3187-4F6C-B38B-685ECA80A3FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E28798-6A14-477D-A561-948A9465FA05}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1282,7 +1282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FBACA70-D51B-4F39-BFB5-0CFDD75735B5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>

</xml_diff>